<commit_message>
no streams for results upload
</commit_message>
<xml_diff>
--- a/apps/static/uploads/filtered_results_template_10.xlsx
+++ b/apps/static/uploads/filtered_results_template_10.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isiahw\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25D3B409-6CA6-450C-B866-B0FCFD634224}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1866581D-9C14-4913-9A8B-66A804E98CC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="95">
   <si>
     <t>reg_no</t>
   </si>
@@ -50,25 +50,22 @@
     <t>notes</t>
   </si>
   <si>
-    <t>Subject</t>
-  </si>
-  <si>
-    <t>Mark</t>
-  </si>
-  <si>
-    <t>12min</t>
-  </si>
-  <si>
-    <t>zosh</t>
-  </si>
-  <si>
-    <t>mine</t>
-  </si>
-  <si>
-    <t>gaka</t>
-  </si>
-  <si>
-    <t>Primary 1</t>
+    <t>subject</t>
+  </si>
+  <si>
+    <t>mark</t>
+  </si>
+  <si>
+    <t>REG007</t>
+  </si>
+  <si>
+    <t>NAMAYANJA</t>
+  </si>
+  <si>
+    <t>MUGERA RITAH</t>
+  </si>
+  <si>
+    <t>Primary 4</t>
   </si>
   <si>
     <t>Term 2</t>
@@ -80,7 +77,199 @@
     <t>2025</t>
   </si>
   <si>
-    <t>BAKING</t>
+    <t>REG058</t>
+  </si>
+  <si>
+    <t>NAKIBUUKA</t>
+  </si>
+  <si>
+    <t>SSANYU FRANCISCA</t>
+  </si>
+  <si>
+    <t>REG062</t>
+  </si>
+  <si>
+    <t>NAMWANJE</t>
+  </si>
+  <si>
+    <t>FORTUNATE</t>
+  </si>
+  <si>
+    <t>REG066</t>
+  </si>
+  <si>
+    <t>NAMALE</t>
+  </si>
+  <si>
+    <t>ZABIBU</t>
+  </si>
+  <si>
+    <t>REG070</t>
+  </si>
+  <si>
+    <t>NAMULINDWA</t>
+  </si>
+  <si>
+    <t>TRACY</t>
+  </si>
+  <si>
+    <t>REG074</t>
+  </si>
+  <si>
+    <t>NAKAZIBWE</t>
+  </si>
+  <si>
+    <t>MARIA ASSUMPTA</t>
+  </si>
+  <si>
+    <t>REG078</t>
+  </si>
+  <si>
+    <t>ATURINDA</t>
+  </si>
+  <si>
+    <t>PRISCILLA</t>
+  </si>
+  <si>
+    <t>REG082</t>
+  </si>
+  <si>
+    <t>KIRWANA</t>
+  </si>
+  <si>
+    <t>HAIRAH BINT YUSUF</t>
+  </si>
+  <si>
+    <t>REG104</t>
+  </si>
+  <si>
+    <t>NAYIGA</t>
+  </si>
+  <si>
+    <t>MARIA ROSETTE</t>
+  </si>
+  <si>
+    <t>REG107</t>
+  </si>
+  <si>
+    <t>KARRIAH</t>
+  </si>
+  <si>
+    <t>BLESSING KIDOCHWUKU</t>
+  </si>
+  <si>
+    <t>REG054</t>
+  </si>
+  <si>
+    <t>BETTY</t>
+  </si>
+  <si>
+    <t>REG051</t>
+  </si>
+  <si>
+    <t>NAMBALIRWA</t>
+  </si>
+  <si>
+    <t>PROSSY</t>
+  </si>
+  <si>
+    <t>REG047</t>
+  </si>
+  <si>
+    <t>KAGABA</t>
+  </si>
+  <si>
+    <t>SELINA</t>
+  </si>
+  <si>
+    <t>REG011</t>
+  </si>
+  <si>
+    <t>AVRIL</t>
+  </si>
+  <si>
+    <t>ELIZABETH KIZITO</t>
+  </si>
+  <si>
+    <t>REG015</t>
+  </si>
+  <si>
+    <t>AHUMUZA</t>
+  </si>
+  <si>
+    <t>GIANNA MAGARA</t>
+  </si>
+  <si>
+    <t>REG019</t>
+  </si>
+  <si>
+    <t>LUYIGA</t>
+  </si>
+  <si>
+    <t>HAGAI</t>
+  </si>
+  <si>
+    <t>REG023</t>
+  </si>
+  <si>
+    <t>NANYONJO</t>
+  </si>
+  <si>
+    <t>RUTH</t>
+  </si>
+  <si>
+    <t>REG027</t>
+  </si>
+  <si>
+    <t>NASSAKA</t>
+  </si>
+  <si>
+    <t>MARIA CATHERINE</t>
+  </si>
+  <si>
+    <t>REG031</t>
+  </si>
+  <si>
+    <t>KEMBABAZI</t>
+  </si>
+  <si>
+    <t>NERIA</t>
+  </si>
+  <si>
+    <t>REG035</t>
+  </si>
+  <si>
+    <t>NAKAWUNDE</t>
+  </si>
+  <si>
+    <t>MARY CATHY</t>
+  </si>
+  <si>
+    <t>REG039</t>
+  </si>
+  <si>
+    <t>NABUKENYA</t>
+  </si>
+  <si>
+    <t>DESIRE</t>
+  </si>
+  <si>
+    <t>REG043</t>
+  </si>
+  <si>
+    <t>NAKYEYUNE</t>
+  </si>
+  <si>
+    <t>JACKIE</t>
+  </si>
+  <si>
+    <t>REG110</t>
+  </si>
+  <si>
+    <t>NACHWA</t>
+  </si>
+  <si>
+    <t>REGINA</t>
   </si>
   <si>
     <t>reg_nos</t>
@@ -101,7 +290,10 @@
     <t>subjects</t>
   </si>
   <si>
-    <t>mine, P1 East, P1 West, P2 E, P2 W, P3 E, P3 W, P4 East, P4 West, P5 East, P5 West, P6 East, P6 West, P7 East, P7 West, Primary 1, PRIMARY 7, PRIMARY FOUR</t>
+    <t>REG007, REG058, REG062, REG066, REG070, REG074, REG078, REG082, REG104, REG107, REG054, REG051, REG047, REG011, REG015, REG019, REG023, REG027, REG031, REG035, REG039, REG043, REG110</t>
+  </si>
+  <si>
+    <t>Primary 4, Primary 5, Primary 6, Primary 7</t>
   </si>
   <si>
     <t>BOT Exam, Final Exam, Midterm Exam, Week 1 Assessment, Week 2 Assessment</t>
@@ -113,7 +305,7 @@
     <t>ART AND DESIGN, BAKING, COMPPREHENSION, COMPUTER, ENGLISH, LIBRARY, LITERACY A, LITERACY B, MATHEMATICS, MUSIC, PHYSICAL EDUCATION, READING, REGIUOS EDUCATION, Science, SEWING, SOCIAL STUDIES</t>
   </si>
   <si>
-    <t>null</t>
+    <t>SOCIAL STUDIES</t>
   </si>
 </sst>
 </file>
@@ -453,22 +645,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.7265625" customWidth="1"/>
-    <col min="2" max="2" width="18.453125" customWidth="1"/>
-    <col min="3" max="3" width="20.81640625" customWidth="1"/>
-    <col min="4" max="4" width="16.81640625" customWidth="1"/>
-    <col min="5" max="5" width="17.90625" customWidth="1"/>
-    <col min="6" max="6" width="15.08984375" customWidth="1"/>
-    <col min="7" max="7" width="14.08984375" customWidth="1"/>
-    <col min="8" max="8" width="14.453125" customWidth="1"/>
+    <col min="10" max="10" width="17.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
@@ -516,46 +701,678 @@
       <c r="C2" t="s">
         <v>13</v>
       </c>
-      <c r="D2" t="s">
-        <v>14</v>
-      </c>
       <c r="E2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" t="s">
+        <v>94</v>
+      </c>
+      <c r="K2">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>18</v>
       </c>
-      <c r="I2" t="s">
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" t="s">
+        <v>94</v>
+      </c>
+      <c r="K3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" t="s">
+        <v>94</v>
+      </c>
+      <c r="K4">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J5" t="s">
+        <v>94</v>
+      </c>
+      <c r="K5">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J6" t="s">
+        <v>94</v>
+      </c>
+      <c r="K6">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>30</v>
       </c>
-      <c r="J2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K2">
+      <c r="B7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" t="s">
+        <v>17</v>
+      </c>
+      <c r="J7" t="s">
+        <v>94</v>
+      </c>
+      <c r="K7">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J8" t="s">
+        <v>94</v>
+      </c>
+      <c r="K8">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" t="s">
+        <v>17</v>
+      </c>
+      <c r="J9" t="s">
+        <v>94</v>
+      </c>
+      <c r="K9">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J10" t="s">
+        <v>94</v>
+      </c>
+      <c r="K10">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" t="s">
+        <v>16</v>
+      </c>
+      <c r="H11" t="s">
+        <v>17</v>
+      </c>
+      <c r="J11" t="s">
+        <v>94</v>
+      </c>
+      <c r="K11">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E12" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12" t="s">
+        <v>16</v>
+      </c>
+      <c r="H12" t="s">
+        <v>17</v>
+      </c>
+      <c r="J12" t="s">
+        <v>94</v>
+      </c>
+      <c r="K12">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" t="s">
+        <v>49</v>
+      </c>
+      <c r="E13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13" t="s">
+        <v>15</v>
+      </c>
+      <c r="G13" t="s">
+        <v>16</v>
+      </c>
+      <c r="H13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J13" t="s">
+        <v>94</v>
+      </c>
+      <c r="K13">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" t="s">
+        <v>52</v>
+      </c>
+      <c r="E14" t="s">
+        <v>14</v>
+      </c>
+      <c r="F14" t="s">
+        <v>15</v>
+      </c>
+      <c r="G14" t="s">
+        <v>16</v>
+      </c>
+      <c r="H14" t="s">
+        <v>17</v>
+      </c>
+      <c r="J14" t="s">
+        <v>94</v>
+      </c>
+      <c r="K14">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" t="s">
+        <v>55</v>
+      </c>
+      <c r="E15" t="s">
+        <v>14</v>
+      </c>
+      <c r="F15" t="s">
+        <v>15</v>
+      </c>
+      <c r="G15" t="s">
+        <v>16</v>
+      </c>
+      <c r="H15" t="s">
+        <v>17</v>
+      </c>
+      <c r="J15" t="s">
+        <v>94</v>
+      </c>
+      <c r="K15">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16" t="s">
+        <v>57</v>
+      </c>
+      <c r="C16" t="s">
+        <v>58</v>
+      </c>
+      <c r="E16" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" t="s">
+        <v>15</v>
+      </c>
+      <c r="G16" t="s">
+        <v>16</v>
+      </c>
+      <c r="H16" t="s">
+        <v>17</v>
+      </c>
+      <c r="J16" t="s">
+        <v>94</v>
+      </c>
+      <c r="K16">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>59</v>
+      </c>
+      <c r="B17" t="s">
+        <v>60</v>
+      </c>
+      <c r="C17" t="s">
+        <v>61</v>
+      </c>
+      <c r="E17" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" t="s">
+        <v>15</v>
+      </c>
+      <c r="G17" t="s">
+        <v>16</v>
+      </c>
+      <c r="H17" t="s">
+        <v>17</v>
+      </c>
+      <c r="J17" t="s">
+        <v>94</v>
+      </c>
+      <c r="K17">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>62</v>
+      </c>
+      <c r="B18" t="s">
+        <v>63</v>
+      </c>
+      <c r="C18" t="s">
+        <v>64</v>
+      </c>
+      <c r="E18" t="s">
+        <v>14</v>
+      </c>
+      <c r="F18" t="s">
+        <v>15</v>
+      </c>
+      <c r="G18" t="s">
+        <v>16</v>
+      </c>
+      <c r="H18" t="s">
+        <v>17</v>
+      </c>
+      <c r="J18" t="s">
+        <v>94</v>
+      </c>
+      <c r="K18">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>65</v>
+      </c>
+      <c r="B19" t="s">
+        <v>66</v>
+      </c>
+      <c r="C19" t="s">
+        <v>67</v>
+      </c>
+      <c r="E19" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" t="s">
+        <v>15</v>
+      </c>
+      <c r="G19" t="s">
+        <v>16</v>
+      </c>
+      <c r="H19" t="s">
+        <v>17</v>
+      </c>
+      <c r="J19" t="s">
+        <v>94</v>
+      </c>
+      <c r="K19">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>68</v>
+      </c>
+      <c r="B20" t="s">
         <v>69</v>
+      </c>
+      <c r="C20" t="s">
+        <v>70</v>
+      </c>
+      <c r="E20" t="s">
+        <v>14</v>
+      </c>
+      <c r="F20" t="s">
+        <v>15</v>
+      </c>
+      <c r="G20" t="s">
+        <v>16</v>
+      </c>
+      <c r="H20" t="s">
+        <v>17</v>
+      </c>
+      <c r="J20" t="s">
+        <v>94</v>
+      </c>
+      <c r="K20">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>71</v>
+      </c>
+      <c r="B21" t="s">
+        <v>72</v>
+      </c>
+      <c r="C21" t="s">
+        <v>73</v>
+      </c>
+      <c r="E21" t="s">
+        <v>14</v>
+      </c>
+      <c r="F21" t="s">
+        <v>15</v>
+      </c>
+      <c r="G21" t="s">
+        <v>16</v>
+      </c>
+      <c r="H21" t="s">
+        <v>17</v>
+      </c>
+      <c r="J21" t="s">
+        <v>94</v>
+      </c>
+      <c r="K21">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>74</v>
+      </c>
+      <c r="B22" t="s">
+        <v>75</v>
+      </c>
+      <c r="C22" t="s">
+        <v>76</v>
+      </c>
+      <c r="E22" t="s">
+        <v>14</v>
+      </c>
+      <c r="F22" t="s">
+        <v>15</v>
+      </c>
+      <c r="G22" t="s">
+        <v>16</v>
+      </c>
+      <c r="H22" t="s">
+        <v>17</v>
+      </c>
+      <c r="J22" t="s">
+        <v>94</v>
+      </c>
+      <c r="K22">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>77</v>
+      </c>
+      <c r="B23" t="s">
+        <v>78</v>
+      </c>
+      <c r="C23" t="s">
+        <v>79</v>
+      </c>
+      <c r="E23" t="s">
+        <v>14</v>
+      </c>
+      <c r="F23" t="s">
+        <v>15</v>
+      </c>
+      <c r="G23" t="s">
+        <v>16</v>
+      </c>
+      <c r="H23" t="s">
+        <v>17</v>
+      </c>
+      <c r="J23" t="s">
+        <v>94</v>
+      </c>
+      <c r="K23">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>80</v>
+      </c>
+      <c r="B24" t="s">
+        <v>81</v>
+      </c>
+      <c r="C24" t="s">
+        <v>82</v>
+      </c>
+      <c r="E24" t="s">
+        <v>14</v>
+      </c>
+      <c r="F24" t="s">
+        <v>15</v>
+      </c>
+      <c r="G24" t="s">
+        <v>16</v>
+      </c>
+      <c r="H24" t="s">
+        <v>17</v>
+      </c>
+      <c r="J24" t="s">
+        <v>94</v>
+      </c>
+      <c r="K24">
+        <v>76</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" sqref="E2" xr:uid="{00000000-0002-0000-0000-000000000000}">
-      <formula1>"mine,P1 East,P1 West,P2 E,P2 W,P3 E,P3 W,P4 East,P4 West,P5 East,P5 West,P6 East,P6 West,P7 East,P7 West,Primary 1,PRIMARY 7,PRIMARY FOUR"</formula1>
+    <dataValidation type="list" allowBlank="1" sqref="E2:E24" xr:uid="{00000000-0002-0000-0000-000000000000}">
+      <formula1>"Primary 4,Primary 5,Primary 6,Primary 7"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="F2" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" sqref="F2:F24" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Term 1,Term 2,Term 3"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="G2" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" sqref="G2:G24" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"BOT Exam,Final Exam,Midterm Exam,Week 1 Assessment,Week 2 Assessment"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="H2" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="list" allowBlank="1" sqref="H2:H24" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"2025"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="J2" xr:uid="{00000000-0002-0000-0000-000004000000}">
+    <dataValidation type="list" allowBlank="1" sqref="J2:J24" xr:uid="{00000000-0002-0000-0000-000004000000}">
       <formula1>"ART AND DESIGN,BAKING,COMPPREHENSION,COMPUTER,ENGLISH,LIBRARY,LITERACY A,LITERACY B,MATHEMATICS,MUSIC,PHYSICAL EDUCATION,READING,REGIUOS EDUCATION,Science,SEWING,SOCIAL STUDIES"</formula1>
     </dataValidation>
   </dataValidations>
@@ -573,42 +1390,42 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>83</v>
       </c>
       <c r="B1" t="s">
-        <v>21</v>
+        <v>84</v>
       </c>
       <c r="C1" t="s">
-        <v>22</v>
+        <v>85</v>
       </c>
       <c r="D1" t="s">
-        <v>23</v>
+        <v>86</v>
       </c>
       <c r="E1" t="s">
-        <v>24</v>
+        <v>87</v>
       </c>
       <c r="F1" t="s">
-        <v>25</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>89</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>90</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>27</v>
+        <v>91</v>
       </c>
       <c r="E2" t="s">
-        <v>28</v>
+        <v>92</v>
       </c>
       <c r="F2" t="s">
-        <v>29</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>